<commit_message>
vram map finished in sheet.c
</commit_message>
<xml_diff>
--- a/MyOS/memory_layout.xlsx
+++ b/MyOS/memory_layout.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA36C795-E7D6-4BFF-83AF-29503B5E928B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D328E86-7F3D-43EB-BF4B-A09D6314B68D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,19 +100,19 @@
     <t>Free Memory</t>
   </si>
   <si>
-    <t>0x00268000 - 0x0026a40f</t>
-  </si>
-  <si>
-    <t>0x0026a410 - 0x0026f7ff</t>
-  </si>
-  <si>
-    <t>9232 B</t>
-  </si>
-  <si>
-    <t>21488 B</t>
-  </si>
-  <si>
     <t>GUI Sheet Controller</t>
+  </si>
+  <si>
+    <t>9236 B</t>
+  </si>
+  <si>
+    <t>0x00268000 - 0x0026a413</t>
+  </si>
+  <si>
+    <t>0x0026a414 - 0x0026f7ff</t>
+  </si>
+  <si>
+    <t>21484 B</t>
   </si>
 </sst>
 </file>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,25 +501,25 @@
     </row>
     <row r="4" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2"/>
     </row>

</xml_diff>

<commit_message>
timer and screen setup finished
</commit_message>
<xml_diff>
--- a/MyOS/memory_layout.xlsx
+++ b/MyOS/memory_layout.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D328E86-7F3D-43EB-BF4B-A09D6314B68D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187DBFEA-CB6E-4371-91FE-6B431740731E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>content</t>
   </si>
@@ -94,9 +94,6 @@
     <t>0x00400000 - 0xdfffffff</t>
   </si>
   <si>
-    <t>3068 MB</t>
-  </si>
-  <si>
     <t>Free Memory</t>
   </si>
   <si>
@@ -109,10 +106,22 @@
     <t>0x00268000 - 0x0026a413</t>
   </si>
   <si>
-    <t>0x0026a414 - 0x0026f7ff</t>
-  </si>
-  <si>
-    <t>21484 B</t>
+    <t>0x0026a414 - 0x0026a41b</t>
+  </si>
+  <si>
+    <t>0x0026a41c - 0x0026f7ff</t>
+  </si>
+  <si>
+    <t>21476 B</t>
+  </si>
+  <si>
+    <t>System Timer</t>
+  </si>
+  <si>
+    <t>8 B</t>
+  </si>
+  <si>
+    <t>&lt;=3068 MB</t>
   </si>
 </sst>
 </file>
@@ -447,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,80 +510,86 @@
     </row>
     <row r="4" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
@@ -583,10 +598,10 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
@@ -599,7 +614,6 @@
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="35.25" x14ac:dyDescent="0.5">
       <c r="A14" s="2"/>

</xml_diff>